<commit_message>
Added quantity & units
</commit_message>
<xml_diff>
--- a/dictionary.xlsx
+++ b/dictionary.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="managers" sheetId="1" r:id="rId1"/>
     <sheet name="products" sheetId="2" r:id="rId2"/>
+    <sheet name="units" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>login</t>
   </si>
@@ -63,6 +64,27 @@
   </si>
   <si>
     <t>ЦЕМ I 42.5Н Беларусь</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>тонн</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>т.</t>
+  </si>
+  <si>
+    <t>т</t>
+  </si>
+  <si>
+    <t>кубов</t>
+  </si>
+  <si>
+    <t>куб</t>
   </si>
 </sst>
 </file>
@@ -429,7 +451,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -477,9 +501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -534,4 +556,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>